<commit_message>
Fix leaderboard to correctly show total participant count for quizzes
Adds postgresql module and corrects totalParticipants count in QuizRankingServiceImpl.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a66e0b79-dc18-4b2d-8a7c-af8ca992d32f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/76358b48-cbc1-499f-982c-0fb145fd4359/09c658b0-ce1b-4d45-ad08-9bad2cd16d6c.jpg
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>2025-04-25 05:26:42</t>
+  </si>
+  <si>
+    <t>I079693</t>
+  </si>
+  <si>
+    <t>2025-04-25 05:40:08</t>
   </si>
 </sst>
 </file>
@@ -132,9 +138,67 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -235,22 +299,22 @@
         <v>14</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>60.0</v>
+        <v>100.0</v>
       </c>
       <c r="E3" t="n" s="0">
         <v>5.0</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>35.0</v>
+        <v>33.0</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restrict Excel download to admins and improve application logging
Implements admin-only access for Excel download via /api/rankings/admin/download/excel and enhances logging with LogDirectoryInitializer, LoggingUtils, and logback-spring.xml.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a66e0b79-dc18-4b2d-8a7c-af8ca992d32f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/76358b48-cbc1-499f-982c-0fb145fd4359/09c658b0-ce1b-4d45-ad08-9bad2cd16d6c.jpg
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>2025-04-25 05:40:08</t>
+  </si>
+  <si>
+    <t>NewUser</t>
+  </si>
+  <si>
+    <t>NEW123</t>
+  </si>
+  <si>
+    <t>2025-04-27 12:35:31</t>
+  </si>
+  <si>
+    <t>2025-04-27 12:56:56</t>
   </si>
 </sst>
 </file>
@@ -138,9 +150,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -223,7 +249,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -267,7 +293,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>11</v>
@@ -293,13 +319,13 @@
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>14</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" t="n" s="0">
         <v>100.0</v>
@@ -311,10 +337,36 @@
         <v>5.0</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>33.0</v>
+        <v>34.0</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>18</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G4" t="n" s="0">
+        <v>35.0</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Participant count plus logging fixes
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>2025-04-27 12:56:56</t>
+  </si>
+  <si>
+    <t>Ajay</t>
+  </si>
+  <si>
+    <t>I05235</t>
+  </si>
+  <si>
+    <t>2025-04-27 13:06:43</t>
   </si>
 </sst>
 </file>
@@ -150,9 +159,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -249,7 +260,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -319,13 +330,13 @@
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D3" t="n" s="0">
         <v>100.0</v>
@@ -337,35 +348,61 @@
         <v>5.0</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>34.0</v>
+        <v>26.0</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n" s="0">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D4" t="n" s="0">
         <v>100.0</v>
       </c>
       <c r="E4" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="G4" t="n" s="0">
+        <v>34.0</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="E5" t="n" s="0">
         <v>1.0</v>
       </c>
-      <c r="F4" t="n" s="0">
+      <c r="F5" t="n" s="0">
         <v>1.0</v>
       </c>
-      <c r="G4" t="n" s="0">
+      <c r="G5" t="n" s="0">
         <v>35.0</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H5" t="s" s="0">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve synchronization of quiz results between Excel and the database
Implements Excel backup, database clearing, and prioritized data loading in JpaQuizRankingService and ExcelQuizResultExporterImpl.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a66e0b79-dc18-4b2d-8a7c-af8ca992d32f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/76358b48-cbc1-499f-982c-0fb145fd4359/09c658b0-ce1b-4d45-ad08-9bad2cd16d6c.jpg
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -159,9 +159,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>

</xml_diff>

<commit_message>
Improve the synchronization process for the Excel quiz result data
Refactored Excel quiz result synchronization to run asynchronously on startup, added backup functionality, and JVM optimizations in run_spring.sh.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a66e0b79-dc18-4b2d-8a7c-af8ca992d32f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/76358b48-cbc1-499f-982c-0fb145fd4359/09c658b0-ce1b-4d45-ad08-9bad2cd16d6c.jpg
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -159,9 +159,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -263,7 +265,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -307,7 +309,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>2.0</v>
+        <v>37.0</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>11</v>
@@ -333,7 +335,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>5.0</v>
+        <v>38.0</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>23</v>
@@ -355,58 +357,6 @@
       </c>
       <c r="H3" t="s" s="0">
         <v>25</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>100.0</v>
-      </c>
-      <c r="E4" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="F4" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <v>34.0</v>
-      </c>
-      <c r="H4" t="s" s="0">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="D5" t="n" s="0">
-        <v>100.0</v>
-      </c>
-      <c r="E5" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="F5" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="G5" t="n" s="0">
-        <v>35.0</v>
-      </c>
-      <c r="H5" t="s" s="0">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve backup system to ensure only the latest results are kept
Implements a backup cleanup mechanism in `ExcelQuizResultExporterImpl.java` to retain only the 3 most recent backup files and fixes H2 DB connection issues.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a66e0b79-dc18-4b2d-8a7c-af8ca992d32f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/76358b48-cbc1-499f-982c-0fb145fd4359/09c658b0-ce1b-4d45-ad08-9bad2cd16d6c.jpg
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -159,9 +159,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>

</xml_diff>

<commit_message>
Improve data handling by exporting and importing quiz results effectively
Exports existing quiz results to db_results.xlsx before importing results from results.xlsx and adds export trigger logic.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a66e0b79-dc18-4b2d-8a7c-af8ca992d32f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/76358b48-cbc1-499f-982c-0fb145fd4359/09c658b0-ce1b-4d45-ad08-9bad2cd16d6c.jpg
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -159,9 +159,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>

</xml_diff>

<commit_message>
Improve application deployment and access configurations for stability
Updates application ports, security profiles and adds admin API endpoint access.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a66e0b79-dc18-4b2d-8a7c-af8ca992d32f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/76358b48-cbc1-499f-982c-0fb145fd4359/09c658b0-ce1b-4d45-ad08-9bad2cd16d6c.jpg
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -159,9 +159,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>

</xml_diff>

<commit_message>
Enhance user interface with modern design and improve database management
Updates UI elements in admin panel and toast notifications, increases leaderboard results and updates H2 database.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: a66e0b79-dc18-4b2d-8a7c-af8ca992d32f
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/76358b48-cbc1-499f-982c-0fb145fd4359/09c658b0-ce1b-4d45-ad08-9bad2cd16d6c.jpg
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>2025-04-27 21:52:00</t>
+  </si>
+  <si>
+    <t>I0796921</t>
+  </si>
+  <si>
+    <t>2025-04-27 23:12:00</t>
   </si>
 </sst>
 </file>
@@ -198,9 +204,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -362,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -510,39 +523,39 @@
     </row>
     <row r="6">
       <c r="A6" t="n" s="0">
-        <v>109.0</v>
+        <v>112.0</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D6" t="n" s="0">
-        <v>40.0</v>
+        <v>60.0</v>
       </c>
       <c r="E6" t="n" s="0">
         <v>5.0</v>
       </c>
       <c r="F6" t="n" s="0">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="G6" t="n" s="0">
         <v>12.0</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n" s="0">
-        <v>110.0</v>
+        <v>109.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D7" t="n" s="0">
         <v>40.0</v>
@@ -554,9 +567,35 @@
         <v>2.0</v>
       </c>
       <c r="G7" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n" s="0">
+        <v>110.0</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D8" t="n" s="0">
+        <v>40.0</v>
+      </c>
+      <c r="E8" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="F8" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="G8" t="n" s="0">
         <v>23.0</v>
       </c>
-      <c r="H7" t="s" s="0">
+      <c r="H8" t="s" s="0">
         <v>35</v>
       </c>
     </row>

</xml_diff>